<commit_message>
Erro de Save nas Cédulas Pt.1
Quando as variáveis eram salvas nas suas respectivas cédulas na planilha, eram todas armazenadas no tipo str, mesmo sendo floats, por isso o Excel tinha uma incompatibilidade com as variáveis adicionadas, assim o erro de tipagem tinha que alterado pelo prórprio usuário. Solucionei parcialmente, já que a interface desta parte do programa está ruim, ainda têm esse erro com as porcentagens que utilizam o símbolo "%" no seu final e a planilha está sendo salva de uma forma errada, tal qual o usuário deve restaurá-la sempre depois de uma alteração feita pelo programa.
</commit_message>
<xml_diff>
--- a/TABELA DE AÇÕES.xlsx
+++ b/TABELA DE AÇÕES.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Atalhos Geral\VScode\CursoHarvard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\VScode\InvestSheet - GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,15 +15,34 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>Indicadores</t>
   </si>
   <si>
+    <t>slce3</t>
+  </si>
+  <si>
+    <t>bbas3</t>
+  </si>
+  <si>
+    <t>BBAS3</t>
+  </si>
+  <si>
+    <t>KLBN11</t>
+  </si>
+  <si>
+    <t>SAPR11</t>
+  </si>
+  <si>
+    <t>UNIP6</t>
+  </si>
+  <si>
     <t>Colunas2</t>
   </si>
   <si>
@@ -54,30 +73,63 @@
     <t>PREÇO</t>
   </si>
   <si>
+    <t>19,30</t>
+  </si>
+  <si>
     <t>ROE</t>
   </si>
   <si>
+    <t>22,13%</t>
+  </si>
+  <si>
+    <t>20,10%</t>
+  </si>
+  <si>
     <t>DIVIDEND YIELD</t>
   </si>
   <si>
+    <t>7,01</t>
+  </si>
+  <si>
+    <t>8,03</t>
+  </si>
+  <si>
     <t>DIV LIQUID / EBITDA</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>P / L</t>
   </si>
   <si>
+    <t>7,44</t>
+  </si>
+  <si>
     <t>P / VP</t>
   </si>
   <si>
+    <t>1,65</t>
+  </si>
+  <si>
     <t>PAYOUT</t>
   </si>
   <si>
     <t>CAGR LUCRO</t>
   </si>
   <si>
+    <t>26,41%</t>
+  </si>
+  <si>
+    <t>25,65%</t>
+  </si>
+  <si>
     <t>CAGR RECEITA</t>
   </si>
   <si>
+    <t>34,00%</t>
+  </si>
+  <si>
     <t>ROE &gt; 10%</t>
   </si>
   <si>
@@ -97,24 +149,6 @@
   </si>
   <si>
     <t>P/VP &gt; 2%</t>
-  </si>
-  <si>
-    <t>SLCE3</t>
-  </si>
-  <si>
-    <t>TAEE11</t>
-  </si>
-  <si>
-    <t>BBAS3</t>
-  </si>
-  <si>
-    <t>KLBN11</t>
-  </si>
-  <si>
-    <t>SAPR11</t>
-  </si>
-  <si>
-    <t>UNIP6</t>
   </si>
 </sst>
 </file>
@@ -158,27 +192,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -186,6 +210,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -198,15 +231,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom"/>
@@ -270,14 +294,14 @@
   <autoFilter ref="A1:P11"/>
   <tableColumns count="16">
     <tableColumn id="1" name="Indicadores"/>
-    <tableColumn id="2" name="SLCE3" dataDxfId="6"/>
-    <tableColumn id="3" name="TAEE11" dataDxfId="5"/>
-    <tableColumn id="4" name="BBAS3" dataDxfId="4"/>
-    <tableColumn id="5" name="KLBN11" dataDxfId="3"/>
-    <tableColumn id="6" name="SAPR11" dataDxfId="2"/>
-    <tableColumn id="9" name="UNIP6" dataDxfId="1"/>
+    <tableColumn id="2" name="SLCE3" dataDxfId="2"/>
+    <tableColumn id="3" name="TAEE11" dataDxfId="0"/>
+    <tableColumn id="4" name="BBAS3" dataDxfId="1"/>
+    <tableColumn id="5" name="KLBN11" dataDxfId="6"/>
+    <tableColumn id="6" name="SAPR11" dataDxfId="5"/>
+    <tableColumn id="9" name="UNIP6" dataDxfId="4"/>
     <tableColumn id="7" name="Colunas2"/>
-    <tableColumn id="8" name="Colunas3" dataDxfId="0"/>
+    <tableColumn id="8" name="Colunas3" dataDxfId="3"/>
     <tableColumn id="10" name="Colunas10"/>
     <tableColumn id="11" name="Colunas11"/>
     <tableColumn id="12" name="Colunas12"/>
@@ -578,18 +602,18 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14" style="5" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="14" style="5" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" style="3" customWidth="1"/>
     <col min="9" max="9" width="14" style="3" customWidth="1"/>
     <col min="10" max="16" width="12.140625" style="3" customWidth="1"/>
@@ -599,188 +623,205 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>31</v>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I2" s="2"/>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+        <v>16</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5">
+        <v>56.97</v>
+      </c>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="I5" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="I6" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="I7" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="5">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="I8" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.99</v>
+      </c>
+      <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="I10" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="I11" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="I11" s="1"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>19</v>
+      <c r="B13" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>20</v>
+      <c r="B14" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>21</v>
+      <c r="B15" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="6"/>
+      <c r="B16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>23</v>
+      <c r="B17" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>24</v>
+      <c r="B18" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>25</v>
+      <c r="B19" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>